<commit_message>
Sredjen .zip za predaju
</commit_message>
<xml_diff>
--- a/Faza I - za predaju/2b Format partner budget - Horizon2020.xlsx
+++ b/Faza I - za predaju/2b Format partner budget - Horizon2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13725" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet ETF" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Subcontracting - budzet'!$B$4:$I$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Travel - budzet'!$B$4:$P$43</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -359,9 +359,6 @@
     <t>Крвни притисак сензор - Опсег притиска: 0 mmHg to 258 mmHg, време одзива: 1 millisecond, тачност: ±1 mmHg</t>
   </si>
   <si>
-    <t>Штампач - ласерски, брзина штампе: 19 страница у минути, месечни обим штампе: 8000 страница</t>
-  </si>
-  <si>
     <t>Мобилни телефон - смарт телефон са основним функционалностима</t>
   </si>
   <si>
@@ -501,6 +498,9 @@
   </si>
   <si>
     <t xml:space="preserve">WP1, WP8 - Адвокатске услуге (поштовање закона, прописа, консултације у вези презентовања пројекта, ауторска права..);                                                                                                                      WP5 - Google cloud - TPU (Tensor Processing Unit) - за побољшано обучавање мрежа;                                                                                                                      WP8 - Израда промотивног материјала (флајери, презентације, анимације, рекламе, приказ пројекта); </t>
+  </si>
+  <si>
+    <t>Штампач и скенер - ласерски, брзина штампе: 19 страница у минути, месечни обим штампе: 8000 страница</t>
   </si>
 </sst>
 </file>
@@ -1002,6 +1002,57 @@
     <xf numFmtId="9" fontId="3" fillId="10" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,57 +1078,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1139,7 +1139,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1218,7 +1218,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1597,52 +1597,52 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="K4" s="73"/>
-      <c r="L4" s="65" t="s">
+      <c r="E4" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="63"/>
+      <c r="L4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
       <c r="O4" s="3">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="70" t="s">
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="87" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="65" t="s">
+      <c r="K5" s="88"/>
+      <c r="L5" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
       <c r="O5" s="3">
         <v>1</v>
       </c>
@@ -1650,22 +1650,22 @@
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="72" t="s">
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="73"/>
-      <c r="L6" s="65" t="s">
+      <c r="K6" s="63"/>
+      <c r="L6" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
       <c r="O6" s="61">
         <v>1</v>
       </c>
@@ -1673,22 +1673,22 @@
       <c r="Q6" s="56"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="65" t="s">
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="63"/>
+      <c r="L7" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="3">
         <v>1</v>
       </c>
@@ -1700,56 +1700,56 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="84"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="84"/>
       <c r="S10" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69" t="s">
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" s="11" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="43" t="s">
         <v>54</v>
       </c>
@@ -1800,11 +1800,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
+      <c r="A14" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
       <c r="D14" s="12">
         <v>6</v>
       </c>
@@ -1853,11 +1853,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
+      <c r="A15" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="12">
         <v>2</v>
       </c>
@@ -1908,11 +1908,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
+      <c r="A16" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="12">
         <v>4</v>
       </c>
@@ -1963,11 +1963,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
-        <v>122</v>
-      </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
+      <c r="A17" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="12">
         <v>7</v>
       </c>
@@ -2020,11 +2020,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
+      <c r="A18" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="12">
         <v>15</v>
       </c>
@@ -2077,11 +2077,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
+      <c r="A19" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="12">
         <v>1</v>
       </c>
@@ -2130,11 +2130,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
+      <c r="A20" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="12">
         <v>1</v>
       </c>
@@ -2185,11 +2185,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
+      <c r="A21" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="12">
         <v>5</v>
       </c>
@@ -2240,11 +2240,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="12">
         <f t="shared" ref="D22:R22" si="4">SUM(D14:D21)</f>
         <v>41</v>
@@ -2365,24 +2365,24 @@
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="75"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
+      <c r="O26" s="77"/>
+      <c r="P26" s="77"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="28"/>
@@ -2423,105 +2423,105 @@
       <c r="P28" s="28"/>
     </row>
     <row r="29" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="83" t="str">
+      <c r="A29" s="70" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant ЕТФ</v>
       </c>
-      <c r="B29" s="84"/>
+      <c r="B29" s="71"/>
       <c r="C29" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="87"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
     </row>
     <row r="30" spans="1:20" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="78"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="30">
         <v>80740</v>
       </c>
-      <c r="D30" s="88" t="s">
-        <v>131</v>
-      </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="74"/>
+      <c r="D30" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
       <c r="Q30" s="56"/>
       <c r="R30" s="56"/>
       <c r="S30" s="27"/>
     </row>
     <row r="31" spans="1:20" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="78"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="30">
         <v>78465</v>
       </c>
-      <c r="D31" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
+      <c r="D31" s="69" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
       <c r="S31" s="27"/>
     </row>
     <row r="32" spans="1:20" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="78"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="30">
         <v>40700</v>
       </c>
-      <c r="D32" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
+      <c r="D32" s="69" t="s">
+        <v>132</v>
+      </c>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
       <c r="S32" s="27"/>
     </row>
     <row r="33" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -2555,95 +2555,95 @@
       <c r="P34" s="33"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="str">
+      <c r="A35" s="70" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B35" s="84"/>
+      <c r="B35" s="71"/>
       <c r="C35" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="85" t="s">
+      <c r="D35" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-      <c r="M35" s="86"/>
-      <c r="N35" s="86"/>
-      <c r="O35" s="86"/>
-      <c r="P35" s="86"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="73"/>
     </row>
     <row r="36" spans="1:19" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="78"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="30">
         <v>90500</v>
       </c>
-      <c r="D36" s="82" t="s">
-        <v>134</v>
-      </c>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
-      <c r="N36" s="74"/>
-      <c r="O36" s="74"/>
-      <c r="P36" s="74"/>
+      <c r="D36" s="68" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="69"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="69"/>
       <c r="S36" s="27"/>
     </row>
     <row r="37" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="78"/>
+      <c r="B37" s="64"/>
       <c r="C37" s="30"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="80"/>
-      <c r="J37" s="80"/>
-      <c r="K37" s="80"/>
-      <c r="L37" s="80"/>
-      <c r="M37" s="80"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="81"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="67"/>
       <c r="S37" s="27"/>
     </row>
     <row r="38" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="78" t="s">
+      <c r="A38" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="78"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="30"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
       <c r="S38" s="27"/>
     </row>
   </sheetData>
@@ -2651,6 +2651,33 @@
     <protectedRange sqref="D14:H21 P14:P21 O6 J14:N21 R14:S21 C30:P38" name="Range1"/>
   </protectedRanges>
   <mergeCells count="43">
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:R10"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="J12:R12"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A26:P26"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="D37:P37"/>
@@ -2667,33 +2694,6 @@
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="D30:P30"/>
     <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A26:P26"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:R10"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="J12:R12"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J6:K6"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="1" priority="1">
@@ -2745,93 +2745,93 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
+      <c r="E3" s="80"/>
+      <c r="F3" s="80"/>
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D4" s="2"/>
-      <c r="E4" s="64" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="72" t="s">
-        <v>117</v>
-      </c>
-      <c r="K4" s="73"/>
-      <c r="L4" s="65" t="s">
+      <c r="E4" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="62" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="63"/>
+      <c r="L4" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
       <c r="O4" s="3">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
-      <c r="E5" s="64" t="s">
+      <c r="E5" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="65"/>
-      <c r="G5" s="65"/>
-      <c r="H5" s="65"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="70" t="s">
+      <c r="F5" s="82"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="87" t="s">
         <v>64</v>
       </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="65" t="s">
+      <c r="K5" s="88"/>
+      <c r="L5" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
       <c r="O5" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D6" s="2"/>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="65"/>
-      <c r="G6" s="65"/>
-      <c r="H6" s="65"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="72"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="65" t="s">
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
       <c r="O6" s="61">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="E7" s="65" t="s">
+      <c r="E7" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="72" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="73"/>
-      <c r="L7" s="65" t="s">
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="K7" s="63"/>
+      <c r="L7" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="3">
         <v>1</v>
       </c>
@@ -2842,56 +2842,56 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
-      <c r="N10" s="67"/>
-      <c r="O10" s="67"/>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="84"/>
+      <c r="O10" s="84"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="84"/>
       <c r="S10" s="5"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="69" t="s">
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
       <c r="S12" s="6"/>
     </row>
     <row r="13" spans="1:19" s="11" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62" t="s">
+      <c r="A13" s="79" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="62"/>
-      <c r="C13" s="62"/>
+      <c r="B13" s="79"/>
+      <c r="C13" s="79"/>
       <c r="D13" s="43" t="s">
         <v>54</v>
       </c>
@@ -2942,11 +2942,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="76" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
+      <c r="A14" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
       <c r="D14" s="12">
         <v>2</v>
       </c>
@@ -3001,11 +3001,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
+      <c r="A15" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" s="74"/>
+      <c r="C15" s="74"/>
       <c r="D15" s="12">
         <v>0</v>
       </c>
@@ -3060,11 +3060,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
+      <c r="A16" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="B16" s="74"/>
+      <c r="C16" s="74"/>
       <c r="D16" s="12">
         <v>0</v>
       </c>
@@ -3119,11 +3119,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
-        <v>122</v>
-      </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
+      <c r="A17" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" s="74"/>
+      <c r="C17" s="74"/>
       <c r="D17" s="12">
         <v>1</v>
       </c>
@@ -3178,11 +3178,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
+      <c r="A18" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="74"/>
+      <c r="C18" s="74"/>
       <c r="D18" s="12">
         <v>7</v>
       </c>
@@ -3237,11 +3237,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="76" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
+      <c r="A19" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
       <c r="D19" s="12">
         <v>0</v>
       </c>
@@ -3296,11 +3296,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
+      <c r="A20" s="74" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="74"/>
+      <c r="C20" s="74"/>
       <c r="D20" s="12">
         <v>0</v>
       </c>
@@ -3355,11 +3355,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" s="76"/>
-      <c r="C21" s="76"/>
+      <c r="A21" s="74" t="s">
+        <v>125</v>
+      </c>
+      <c r="B21" s="74"/>
+      <c r="C21" s="74"/>
       <c r="D21" s="12">
         <v>2</v>
       </c>
@@ -3414,11 +3414,11 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="B22" s="77"/>
-      <c r="C22" s="77"/>
+      <c r="B22" s="78"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="12">
         <f t="shared" ref="D22:Q22" si="4">SUM(D14:D21)</f>
         <v>12</v>
@@ -3538,24 +3538,24 @@
       <c r="S25" s="27"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="75"/>
-      <c r="C26" s="75"/>
-      <c r="D26" s="75"/>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
-      <c r="I26" s="75"/>
-      <c r="J26" s="75"/>
-      <c r="K26" s="75"/>
-      <c r="L26" s="75"/>
-      <c r="M26" s="75"/>
-      <c r="N26" s="75"/>
-      <c r="O26" s="75"/>
-      <c r="P26" s="75"/>
+      <c r="B26" s="77"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="77"/>
+      <c r="J26" s="77"/>
+      <c r="K26" s="77"/>
+      <c r="L26" s="77"/>
+      <c r="M26" s="77"/>
+      <c r="N26" s="77"/>
+      <c r="O26" s="77"/>
+      <c r="P26" s="77"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="57"/>
@@ -3596,103 +3596,103 @@
       <c r="P28" s="57"/>
     </row>
     <row r="29" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="83" t="str">
+      <c r="A29" s="70" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B29" s="84"/>
+      <c r="B29" s="71"/>
       <c r="C29" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="76" t="s">
+      <c r="D29" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
-      <c r="I29" s="87"/>
-      <c r="J29" s="87"/>
-      <c r="K29" s="87"/>
-      <c r="L29" s="87"/>
-      <c r="M29" s="87"/>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="87"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
+      <c r="J29" s="75"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="75"/>
+      <c r="M29" s="75"/>
+      <c r="N29" s="75"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
     </row>
     <row r="30" spans="1:20" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="78" t="s">
+      <c r="A30" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="78"/>
+      <c r="B30" s="64"/>
       <c r="C30" s="30">
         <v>26820</v>
       </c>
-      <c r="D30" s="88" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
-      <c r="M30" s="74"/>
-      <c r="N30" s="74"/>
-      <c r="O30" s="74"/>
-      <c r="P30" s="74"/>
+      <c r="D30" s="76" t="s">
+        <v>126</v>
+      </c>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
       <c r="S30" s="27"/>
     </row>
     <row r="31" spans="1:20" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="78" t="s">
+      <c r="A31" s="64" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="78"/>
+      <c r="B31" s="64"/>
       <c r="C31" s="30">
         <v>159310</v>
       </c>
-      <c r="D31" s="74" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="74"/>
-      <c r="K31" s="74"/>
-      <c r="L31" s="74"/>
-      <c r="M31" s="74"/>
-      <c r="N31" s="74"/>
-      <c r="O31" s="74"/>
-      <c r="P31" s="74"/>
+      <c r="D31" s="69" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
       <c r="S31" s="27"/>
     </row>
     <row r="32" spans="1:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="78" t="s">
+      <c r="A32" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="78"/>
+      <c r="B32" s="64"/>
       <c r="C32" s="30">
         <v>9500</v>
       </c>
-      <c r="D32" s="74" t="s">
-        <v>129</v>
-      </c>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="74"/>
-      <c r="K32" s="74"/>
-      <c r="L32" s="74"/>
-      <c r="M32" s="74"/>
-      <c r="N32" s="74"/>
-      <c r="O32" s="74"/>
-      <c r="P32" s="74"/>
+      <c r="D32" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
       <c r="S32" s="27"/>
     </row>
     <row r="33" spans="1:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -3726,95 +3726,95 @@
       <c r="P34" s="33"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="83" t="str">
+      <c r="A35" s="70" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B35" s="84"/>
+      <c r="B35" s="71"/>
       <c r="C35" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="85" t="s">
+      <c r="D35" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="86"/>
-      <c r="I35" s="86"/>
-      <c r="J35" s="86"/>
-      <c r="K35" s="86"/>
-      <c r="L35" s="86"/>
-      <c r="M35" s="86"/>
-      <c r="N35" s="86"/>
-      <c r="O35" s="86"/>
-      <c r="P35" s="86"/>
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="73"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="73"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="73"/>
+      <c r="O35" s="73"/>
+      <c r="P35" s="73"/>
     </row>
     <row r="36" spans="1:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="78" t="s">
+      <c r="A36" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="78"/>
+      <c r="B36" s="64"/>
       <c r="C36" s="30">
         <v>87500</v>
       </c>
-      <c r="D36" s="82" t="s">
-        <v>130</v>
-      </c>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="74"/>
-      <c r="J36" s="74"/>
-      <c r="K36" s="74"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
-      <c r="N36" s="74"/>
-      <c r="O36" s="74"/>
-      <c r="P36" s="74"/>
+      <c r="D36" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="E36" s="69"/>
+      <c r="F36" s="69"/>
+      <c r="G36" s="69"/>
+      <c r="H36" s="69"/>
+      <c r="I36" s="69"/>
+      <c r="J36" s="69"/>
+      <c r="K36" s="69"/>
+      <c r="L36" s="69"/>
+      <c r="M36" s="69"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="69"/>
       <c r="S36" s="27"/>
     </row>
     <row r="37" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="78" t="s">
+      <c r="A37" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="78"/>
+      <c r="B37" s="64"/>
       <c r="C37" s="30"/>
-      <c r="D37" s="79"/>
-      <c r="E37" s="80"/>
-      <c r="F37" s="80"/>
-      <c r="G37" s="80"/>
-      <c r="H37" s="80"/>
-      <c r="I37" s="80"/>
-      <c r="J37" s="80"/>
-      <c r="K37" s="80"/>
-      <c r="L37" s="80"/>
-      <c r="M37" s="80"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="80"/>
-      <c r="P37" s="81"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="67"/>
       <c r="S37" s="27"/>
     </row>
     <row r="38" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="78" t="s">
+      <c r="A38" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="B38" s="78"/>
+      <c r="B38" s="64"/>
       <c r="C38" s="30"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="74"/>
-      <c r="J38" s="74"/>
-      <c r="K38" s="74"/>
-      <c r="L38" s="74"/>
-      <c r="M38" s="74"/>
-      <c r="N38" s="74"/>
-      <c r="O38" s="74"/>
-      <c r="P38" s="74"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="69"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="69"/>
+      <c r="O38" s="69"/>
+      <c r="P38" s="69"/>
       <c r="S38" s="27"/>
     </row>
   </sheetData>
@@ -3823,19 +3823,24 @@
     <protectedRange sqref="D18:H18" name="Range1_1"/>
   </protectedRanges>
   <mergeCells count="43">
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:P36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D35:P35"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A26:P26"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:P29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:P30"/>
     <mergeCell ref="A21:C21"/>
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
@@ -3848,24 +3853,19 @@
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A26:P26"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:P29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:P30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D35:P35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:P36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:N5"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -3887,7 +3887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
@@ -4195,7 +4195,7 @@
     </row>
     <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="47"/>
       <c r="D11" s="49" t="s">
@@ -4208,7 +4208,7 @@
         <v>58</v>
       </c>
       <c r="G11" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H11" s="47">
         <v>1</v>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="47"/>
       <c r="D12" s="49" t="s">
@@ -4250,7 +4250,7 @@
         <v>65</v>
       </c>
       <c r="G12" s="47" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
@@ -4277,7 +4277,7 @@
     </row>
     <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C13" s="47"/>
       <c r="D13" s="49" t="s">
@@ -4290,7 +4290,7 @@
         <v>58</v>
       </c>
       <c r="G13" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" s="47">
         <v>1</v>
@@ -4319,7 +4319,7 @@
     </row>
     <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" s="47"/>
       <c r="D14" s="49" t="s">
@@ -4332,7 +4332,7 @@
         <v>65</v>
       </c>
       <c r="G14" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H14" s="47"/>
       <c r="I14" s="47"/>
@@ -4357,7 +4357,7 @@
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" s="47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>76</v>
@@ -4372,7 +4372,7 @@
         <v>69</v>
       </c>
       <c r="G15" s="47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H15" s="47">
         <v>1</v>
@@ -5132,7 +5132,7 @@
         <v>69</v>
       </c>
       <c r="G33" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H33" s="47">
         <v>1</v>
@@ -5174,7 +5174,7 @@
         <v>74</v>
       </c>
       <c r="G34" s="47" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H34" s="47">
         <v>1</v>
@@ -5216,7 +5216,7 @@
         <v>69</v>
       </c>
       <c r="G35" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H35" s="47">
         <v>2</v>
@@ -5262,7 +5262,7 @@
         <v>67</v>
       </c>
       <c r="G36" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H36" s="51"/>
       <c r="I36" s="51"/>
@@ -5300,7 +5300,7 @@
         <v>74</v>
       </c>
       <c r="G37" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H37" s="47">
         <v>1</v>
@@ -6004,8 +6004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6091,7 +6091,7 @@
         <v>68</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G6" s="34">
         <v>200</v>
@@ -6116,7 +6116,7 @@
         <v>68</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="34">
         <v>60</v>
@@ -6141,7 +6141,7 @@
         <v>68</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G8" s="55">
         <v>3000</v>
@@ -6193,7 +6193,7 @@
         <v>84</v>
       </c>
       <c r="F10" s="42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="53">
         <v>12825</v>
@@ -6218,7 +6218,7 @@
         <v>73</v>
       </c>
       <c r="F11" s="54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G11" s="54">
         <v>12825</v>
@@ -6243,7 +6243,7 @@
         <v>66</v>
       </c>
       <c r="F12" s="54" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G12" s="54">
         <v>1600</v>
@@ -6270,7 +6270,7 @@
         <v>84</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G13" s="34">
         <v>1600</v>
@@ -6295,7 +6295,7 @@
         <v>73</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G14" s="34">
         <v>1600</v>
@@ -6322,7 +6322,7 @@
         <v>84</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G15" s="34">
         <v>250</v>
@@ -6349,7 +6349,7 @@
         <v>84</v>
       </c>
       <c r="F16" s="34" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G16" s="34">
         <v>900</v>
@@ -6374,7 +6374,7 @@
         <v>68</v>
       </c>
       <c r="F17" s="44" t="s">
-        <v>87</v>
+        <v>134</v>
       </c>
       <c r="G17" s="44">
         <v>120</v>
@@ -6399,7 +6399,7 @@
         <v>73</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G18" s="53">
         <v>99700</v>
@@ -6424,7 +6424,7 @@
         <v>59</v>
       </c>
       <c r="F19" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G19" s="34">
         <v>99700</v>
@@ -6451,7 +6451,7 @@
         <v>84</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G20" s="34">
         <v>6155</v>
@@ -6476,7 +6476,7 @@
         <v>68</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G21" s="34">
         <v>2855</v>
@@ -6491,17 +6491,17 @@
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E22" s="34" t="s">
         <v>71</v>
       </c>
       <c r="F22" s="34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G22" s="34">
         <v>8400</v>
@@ -6516,7 +6516,7 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C23" s="34"/>
       <c r="D23" s="54" t="s">
@@ -6526,7 +6526,7 @@
         <v>66</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G23" s="34">
         <v>1750</v>
@@ -6551,7 +6551,7 @@
         <v>66</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G24" s="34">
         <v>47500</v>
@@ -6787,7 +6787,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" s="52" t="s">
         <v>76</v>
@@ -6799,7 +6799,7 @@
         <v>84</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" s="52">
         <v>30000</v>
@@ -6824,7 +6824,7 @@
         <v>73</v>
       </c>
       <c r="F6" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="52">
         <v>10000</v>
@@ -6849,7 +6849,7 @@
         <v>68</v>
       </c>
       <c r="F7" s="52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" s="52">
         <v>10000</v>
@@ -6876,7 +6876,7 @@
         <v>84</v>
       </c>
       <c r="F8" s="52" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G8" s="52">
         <v>2000</v>
@@ -6901,7 +6901,7 @@
         <v>68</v>
       </c>
       <c r="F9" s="52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G9" s="52">
         <v>25000</v>
@@ -6928,7 +6928,7 @@
         <v>84</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" s="34">
         <v>58500</v>
@@ -6953,7 +6953,7 @@
         <v>73</v>
       </c>
       <c r="F11" s="53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G11" s="53">
         <v>58500</v>
@@ -6978,7 +6978,7 @@
         <v>73</v>
       </c>
       <c r="F12" s="46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G12" s="46">
         <v>9500</v>

</xml_diff>